<commit_message>
A lot of 1.1 features being added
</commit_message>
<xml_diff>
--- a/Excel Workbooks/level unlocks.xlsx
+++ b/Excel Workbooks/level unlocks.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Dropbox\USB Drive\Daniel\Programming\C#\Gaming\Games\OneCannonOneArmy\Excel Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Backed Up Games\OneCannonOneArmy\Excel Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840E88D5-5862-4ED4-8080-CED01C380B04}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="2760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Level</t>
   </si>
@@ -47,9 +48,6 @@
     <t>Defense Aliens, Hammer</t>
   </si>
   <si>
-    <t>Light Poison Resistant Aliens</t>
-  </si>
-  <si>
     <t>Fireball, Light Fire Defense Aliens, Snowball</t>
   </si>
   <si>
@@ -86,9 +84,6 @@
     <t>Plasma-Resistant Alien</t>
   </si>
   <si>
-    <t>Absorb Hex</t>
-  </si>
-  <si>
     <t>Laser, Omega Alien</t>
   </si>
   <si>
@@ -101,22 +96,19 @@
     <t>Fire Defense Aliens, Ice Shard</t>
   </si>
   <si>
-    <t>Cursed Rocket</t>
-  </si>
-  <si>
-    <t>Plasma Hex</t>
-  </si>
-  <si>
     <t>Hex, Ninja Aliens</t>
   </si>
   <si>
     <t>Lightning, Freeze-Proof Aliens, Frost Hex</t>
+  </si>
+  <si>
+    <t>Light Poison Resistant Aliens, Absorb Hex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,11 +446,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -520,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -540,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -570,7 +562,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -580,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -590,7 +582,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -600,7 +592,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -610,7 +602,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -620,7 +612,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -630,7 +622,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -640,7 +632,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -650,11 +642,9 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -662,11 +652,9 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -674,7 +662,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -684,7 +672,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -694,7 +682,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2"/>
     </row>
@@ -704,7 +692,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="2"/>
     </row>
@@ -713,18 +701,16 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +719,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="2"/>
     </row>

</xml_diff>